<commit_message>
measuring average complexity of a project
</commit_message>
<xml_diff>
--- a/MatrixData.xlsx
+++ b/MatrixData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\paperwork\tscomplexity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078878A8-8B58-4B97-9A4D-85956C85D7A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAD74BC-D5FA-4862-888E-FE39CD5576A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{75C10C4B-DB93-4ED3-9A05-ED399035CC8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="3" xr2:uid="{75C10C4B-DB93-4ED3-9A05-ED399035CC8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Average_cyclomatic" sheetId="1" r:id="rId1"/>
     <sheet name="Comment_ratio" sheetId="2" r:id="rId2"/>
     <sheet name="NOS" sheetId="3" r:id="rId3"/>
+    <sheet name="NOF" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t>Connect-four</t>
   </si>
@@ -1137,67 +1138,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of Statements of the projects</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1621,6 +1562,444 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NOF!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JavaScript</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>NOF!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Connect-four</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gomoku</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tetris</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mario-dodger</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Video Player</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Audio Player</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Video to MP3 Converter</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shareit</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Messenger</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Video downloader</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NOF!$C$3:$L$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D0DA-4340-B52A-C4DEE55EDE59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NOF!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TypeScript</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>NOF!$C$2:$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Connect-four</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gomoku</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tetris</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Mario-dodger</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Video Player</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Audio Player</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Video to MP3 Converter</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Shareit</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Messenger</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Video downloader</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NOF!$C$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D0DA-4340-B52A-C4DEE55EDE59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1216608751"/>
+        <c:axId val="1332483407"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1216608751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332483407"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1332483407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1216608751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1741,6 +2120,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2748,6 +3167,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3353,6 +4275,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F49594FD-FF5D-4D53-97A7-B296E92ABD54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D78B53F-F75A-456D-8FEF-EC8AEBF739DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3672,8 +4635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689DF251-24B1-481C-8295-08DABE480953}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,7 +4763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A771E1B3-5019-4746-83A9-D1A909B15883}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -3930,8 +4893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3DED70-1BF6-4B38-AB55-964A1B51E9C7}">
   <dimension ref="A2:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,4 +5018,134 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11A3FA9-3DF6-44A8-8F25-9BB8AD0618CA}">
+  <dimension ref="B2:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>204</v>
+      </c>
+      <c r="F3">
+        <v>1124</v>
+      </c>
+      <c r="G3">
+        <v>98</v>
+      </c>
+      <c r="H3">
+        <v>214</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>429</v>
+      </c>
+      <c r="K3">
+        <v>429</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>113</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>232</v>
+      </c>
+      <c r="H4">
+        <v>232</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>162</v>
+      </c>
+      <c r="K4">
+        <v>185</v>
+      </c>
+      <c r="L4">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>